<commit_message>
Recovered Myxicola sp.A and sp.B which were mysteriously axed in a version management conflict
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Annelida.xlsx
+++ b/data/dataPaper-I-in/arphified/Annelida.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="456">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -537,7 +537,7 @@
     <t>(Kinberg, 1866)</t>
   </si>
   <si>
-    <t>49534</t>
+    <t>492594</t>
   </si>
   <si>
     <t>Myxicola</t>
@@ -550,6 +550,9 @@
   </si>
   <si>
     <t>Myxicola sp.A = "Myxicola aesthetica"; In Europe, M. infundibulum is found in soft-sediments and M. aesthetica on docks &amp; hard-surfaces. However, specimens from the NEP are morphologically and genetically different. In the past, several species of Myxicola were described from California, Puget Sound, and Alaska. This material needs to be re-examined.</t>
+  </si>
+  <si>
+    <t>49533</t>
   </si>
   <si>
     <t>sp.B</t>
@@ -4879,7 +4882,7 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
@@ -4936,7 +4939,7 @@
         <v>36</v>
       </c>
       <c r="T31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="U31" t="s">
         <v>36</v>
@@ -4978,12 +4981,12 @@
         <v>36</v>
       </c>
       <c r="AH31" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
@@ -5034,13 +5037,13 @@
         <v>36</v>
       </c>
       <c r="R32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S32" t="s">
         <v>36</v>
       </c>
       <c r="T32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="U32" t="s">
         <v>36</v>
@@ -5052,7 +5055,7 @@
         <v>36</v>
       </c>
       <c r="X32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="Y32" t="s">
         <v>36</v>
@@ -5087,7 +5090,7 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
@@ -5138,13 +5141,13 @@
         <v>36</v>
       </c>
       <c r="R33" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S33" t="s">
         <v>36</v>
       </c>
       <c r="T33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="U33" t="s">
         <v>36</v>
@@ -5191,7 +5194,7 @@
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -5242,13 +5245,13 @@
         <v>36</v>
       </c>
       <c r="R34" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="S34" t="s">
         <v>36</v>
       </c>
       <c r="T34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="U34" t="s">
         <v>36</v>
@@ -5260,7 +5263,7 @@
         <v>36</v>
       </c>
       <c r="X34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="Y34" t="s">
         <v>36</v>
@@ -5295,7 +5298,7 @@
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -5334,7 +5337,7 @@
         <v>36</v>
       </c>
       <c r="N35" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O35" t="s">
         <v>36</v>
@@ -5346,13 +5349,13 @@
         <v>36</v>
       </c>
       <c r="R35" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="S35" t="s">
         <v>36</v>
       </c>
       <c r="T35" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="U35" t="s">
         <v>36</v>
@@ -5364,7 +5367,7 @@
         <v>36</v>
       </c>
       <c r="X35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Y35" t="s">
         <v>36</v>
@@ -5399,7 +5402,7 @@
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -5438,7 +5441,7 @@
         <v>36</v>
       </c>
       <c r="N36" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O36" t="s">
         <v>36</v>
@@ -5450,13 +5453,13 @@
         <v>36</v>
       </c>
       <c r="R36" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S36" t="s">
         <v>36</v>
       </c>
       <c r="T36" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="U36" t="s">
         <v>36</v>
@@ -5503,7 +5506,7 @@
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -5542,7 +5545,7 @@
         <v>36</v>
       </c>
       <c r="N37" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O37" t="s">
         <v>36</v>
@@ -5554,7 +5557,7 @@
         <v>36</v>
       </c>
       <c r="R37" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="S37" t="s">
         <v>36</v>
@@ -5572,7 +5575,7 @@
         <v>36</v>
       </c>
       <c r="X37" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="Y37" t="s">
         <v>36</v>
@@ -5607,7 +5610,7 @@
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B38" t="s">
         <v>35</v>
@@ -5646,7 +5649,7 @@
         <v>36</v>
       </c>
       <c r="N38" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O38" t="s">
         <v>36</v>
@@ -5658,13 +5661,13 @@
         <v>36</v>
       </c>
       <c r="R38" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="S38" t="s">
         <v>36</v>
       </c>
       <c r="T38" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="U38" t="s">
         <v>36</v>
@@ -5676,7 +5679,7 @@
         <v>36</v>
       </c>
       <c r="X38" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Y38" t="s">
         <v>36</v>
@@ -5711,7 +5714,7 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
@@ -5750,7 +5753,7 @@
         <v>36</v>
       </c>
       <c r="N39" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O39" t="s">
         <v>36</v>
@@ -5762,13 +5765,13 @@
         <v>36</v>
       </c>
       <c r="R39" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S39" t="s">
         <v>36</v>
       </c>
       <c r="T39" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="U39" t="s">
         <v>36</v>
@@ -5780,7 +5783,7 @@
         <v>36</v>
       </c>
       <c r="X39" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Y39" t="s">
         <v>36</v>
@@ -5815,7 +5818,7 @@
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
@@ -5854,7 +5857,7 @@
         <v>36</v>
       </c>
       <c r="N40" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O40" t="s">
         <v>36</v>
@@ -5866,13 +5869,13 @@
         <v>36</v>
       </c>
       <c r="R40" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="S40" t="s">
         <v>36</v>
       </c>
       <c r="T40" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="U40" t="s">
         <v>36</v>
@@ -5884,7 +5887,7 @@
         <v>36</v>
       </c>
       <c r="X40" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="Y40" t="s">
         <v>36</v>
@@ -5914,12 +5917,12 @@
         <v>36</v>
       </c>
       <c r="AH40" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B41" t="s">
         <v>35</v>
@@ -5958,25 +5961,25 @@
         <v>36</v>
       </c>
       <c r="N41" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O41" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="P41" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="Q41" t="s">
         <v>36</v>
       </c>
       <c r="R41" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="S41" t="s">
         <v>36</v>
       </c>
       <c r="T41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="U41" t="s">
         <v>36</v>
@@ -6023,7 +6026,7 @@
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B42" t="s">
         <v>35</v>
@@ -6050,10 +6053,10 @@
         <v>36</v>
       </c>
       <c r="J42" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K42" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L42" t="s">
         <v>36</v>
@@ -6062,7 +6065,7 @@
         <v>36</v>
       </c>
       <c r="N42" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O42" t="s">
         <v>36</v>
@@ -6074,13 +6077,13 @@
         <v>36</v>
       </c>
       <c r="R42" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="S42" t="s">
         <v>36</v>
       </c>
       <c r="T42" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="U42" t="s">
         <v>36</v>
@@ -6127,7 +6130,7 @@
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -6154,10 +6157,10 @@
         <v>36</v>
       </c>
       <c r="J43" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K43" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L43" t="s">
         <v>36</v>
@@ -6166,7 +6169,7 @@
         <v>36</v>
       </c>
       <c r="N43" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O43" t="s">
         <v>36</v>
@@ -6178,13 +6181,13 @@
         <v>36</v>
       </c>
       <c r="R43" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="S43" t="s">
         <v>36</v>
       </c>
       <c r="T43" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="U43" t="s">
         <v>36</v>
@@ -6196,7 +6199,7 @@
         <v>36</v>
       </c>
       <c r="X43" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Y43" t="s">
         <v>36</v>
@@ -6226,12 +6229,12 @@
         <v>36</v>
       </c>
       <c r="AH43" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B44" t="s">
         <v>35</v>
@@ -6258,10 +6261,10 @@
         <v>36</v>
       </c>
       <c r="J44" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K44" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L44" t="s">
         <v>36</v>
@@ -6270,7 +6273,7 @@
         <v>36</v>
       </c>
       <c r="N44" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O44" t="s">
         <v>36</v>
@@ -6282,13 +6285,13 @@
         <v>36</v>
       </c>
       <c r="R44" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="S44" t="s">
         <v>36</v>
       </c>
       <c r="T44" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="U44" t="s">
         <v>36</v>
@@ -6300,7 +6303,7 @@
         <v>36</v>
       </c>
       <c r="X44" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="Y44" t="s">
         <v>36</v>
@@ -6330,12 +6333,12 @@
         <v>36</v>
       </c>
       <c r="AH44" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B45" t="s">
         <v>35</v>
@@ -6362,10 +6365,10 @@
         <v>36</v>
       </c>
       <c r="J45" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K45" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L45" t="s">
         <v>36</v>
@@ -6374,10 +6377,10 @@
         <v>36</v>
       </c>
       <c r="N45" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O45" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P45" t="s">
         <v>36</v>
@@ -6386,13 +6389,13 @@
         <v>36</v>
       </c>
       <c r="R45" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="S45" t="s">
         <v>36</v>
       </c>
       <c r="T45" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="U45" t="s">
         <v>36</v>
@@ -6439,7 +6442,7 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B46" t="s">
         <v>35</v>
@@ -6466,10 +6469,10 @@
         <v>36</v>
       </c>
       <c r="J46" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K46" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L46" t="s">
         <v>36</v>
@@ -6478,10 +6481,10 @@
         <v>36</v>
       </c>
       <c r="N46" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O46" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P46" t="s">
         <v>36</v>
@@ -6490,13 +6493,13 @@
         <v>36</v>
       </c>
       <c r="R46" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="S46" t="s">
         <v>36</v>
       </c>
       <c r="T46" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="U46" t="s">
         <v>36</v>
@@ -6508,7 +6511,7 @@
         <v>36</v>
       </c>
       <c r="X46" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="Y46" t="s">
         <v>36</v>
@@ -6543,7 +6546,7 @@
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -6570,10 +6573,10 @@
         <v>36</v>
       </c>
       <c r="J47" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K47" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L47" t="s">
         <v>36</v>
@@ -6582,10 +6585,10 @@
         <v>36</v>
       </c>
       <c r="N47" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O47" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P47" t="s">
         <v>36</v>
@@ -6594,13 +6597,13 @@
         <v>36</v>
       </c>
       <c r="R47" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="S47" t="s">
         <v>36</v>
       </c>
       <c r="T47" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="U47" t="s">
         <v>36</v>
@@ -6661,495 +6664,495 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="K1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="L1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="M1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="N1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="O1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="P1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="Q1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="R1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="S1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="T1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="U1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="V1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="W1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="X1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="Y1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="Z1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AA1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AB1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AC1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AD1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AE1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AF1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AG1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AH1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AI1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AJ1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AK1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AL1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AM1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AN1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AO1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AP1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AQ1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AR1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AS1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AT1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AU1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AV1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AW1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AX1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AY1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AZ1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="BA1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="BB1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="BC1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="BD1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="BE1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="BF1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="BG1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="BH1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="BI1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="BJ1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="BK1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="BL1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="BM1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="BN1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="BO1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="BP1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="BQ1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="BR1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="BS1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="BT1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="BU1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="BV1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="BW1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="BX1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="BY1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="BZ1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CA1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CB1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CC1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CD1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CE1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CF1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CG1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CH1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CI1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CJ1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CK1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CL1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CM1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CN1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CO1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="CP1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="CQ1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="CR1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="CS1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="CT1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="CU1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="CV1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="CW1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CX1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="CY1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="CZ1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="DA1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="DB1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="DC1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="DD1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="DE1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="DF1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="DG1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="DH1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="DI1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="DJ1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="DK1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="DL1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="DM1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="DN1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="DO1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="DP1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="DQ1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="DR1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="DS1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="DT1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="DU1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="DV1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="DW1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="DX1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="DY1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="DZ1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="EA1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="EB1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="EC1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="ED1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="EE1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="EF1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="EG1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="EH1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="EI1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="EJ1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="EK1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="EL1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="EM1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="EN1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="EO1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="EP1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="EQ1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="ER1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="ES1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="ET1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="EU1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="EV1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="EW1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="EX1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="EY1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="EZ1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="FA1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="FB1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="FC1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="FD1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -7161,428 +7164,428 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="I2" t="s">
         <v>36</v>
       </c>
       <c r="J2" t="s">
+        <v>413</v>
+      </c>
+      <c r="K2" t="s">
+        <v>414</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>416</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
+        <v>417</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>418</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>419</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>420</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>421</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>422</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>423</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>424</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>425</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>426</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>427</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>428</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>429</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>430</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>431</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>432</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>433</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>434</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>435</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>436</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>437</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>438</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>439</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
         <v>412</v>
       </c>
-      <c r="K2" t="s">
-        <v>413</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" t="s">
-        <v>414</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>415</v>
-      </c>
-      <c r="U2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" t="s">
-        <v>416</v>
-      </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>440</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>441</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>442</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>443</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>444</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>445</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>446</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>447</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>448</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>449</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ER2" t="s">
         <v>417</v>
       </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>418</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>419</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>420</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>421</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>422</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>423</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>424</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>425</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>426</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>427</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>428</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>429</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>430</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>431</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>432</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>433</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>434</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>435</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>436</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>437</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>438</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>411</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>439</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>440</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>441</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>442</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>443</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>444</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>445</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>446</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>447</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>448</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>416</v>
-      </c>
       <c r="ES2" t="s">
         <v>36</v>
       </c>
@@ -7593,19 +7596,19 @@
         <v>36</v>
       </c>
       <c r="EV2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="EW2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="EX2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="EY2" t="s">
         <v>36</v>
       </c>
       <c r="EZ2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="FA2" t="s">
         <v>36</v>
@@ -7636,10 +7639,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Possibly final version after correcting Myxicola issue following second review
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Annelida.xlsx
+++ b/data/dataPaper-I-in/arphified/Annelida.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="448">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -462,9 +462,6 @@
     <t>374226</t>
   </si>
   <si>
-    <t>Considering the presence of multiple species of Phyllochaetopterus in the Northeast Pacific, some of which are undescribed, Phyllochaetopterus sp. is here reported.</t>
-  </si>
-  <si>
     <t>552559</t>
   </si>
   <si>
@@ -543,22 +540,22 @@
     <t>Myxicola</t>
   </si>
   <si>
-    <t>sp.A</t>
-  </si>
-  <si>
-    <t>Harris (provisional species name)</t>
-  </si>
-  <si>
-    <t>Myxicola sp.A = "Myxicola aesthetica"; In Europe, M. infundibulum is found in soft-sediments and M. aesthetica on docks &amp; hard-surfaces. However, specimens from the NEP are morphologically and genetically different. In the past, several species of Myxicola were described from California, Puget Sound, and Alaska. This material needs to be re-examined.</t>
+    <t>aff.</t>
+  </si>
+  <si>
+    <t>aesthetica</t>
+  </si>
+  <si>
+    <t>(Myxicola sp.A sensu Leslie Harris, provisional name); In Europe, M. aesthetica is found on docks &amp; hard-surfaces. However, specimens from the NEP that exhibit this habit are morphologically and genetically different. In the past, several species of Myxicola were described from California, Puget Sound, and Alaska. This material needs to be re-examined.</t>
   </si>
   <si>
     <t>49533</t>
   </si>
   <si>
-    <t>sp.B</t>
-  </si>
-  <si>
-    <t>Myxicola sp.B = "Myxicola infundibulum"; In Europe, M. infundibulum is found in soft-sediments and M. aesthetica on docks &amp; hard-surfaces. However, specimens from the NEP are morphologically and genetically different. In the past, several species of Myxicola were described from California, Puget Sound, and Alaska. This material needs to be re-examined.</t>
+    <t>infundibulum</t>
+  </si>
+  <si>
+    <t>(Myxicola sp.B sensu Leslie Harris, provisional name); In Europe, M. infundibulum is found in soft-sediments. However, specimens from the NEP that exhibit this habit are morphologically and genetically different. In the past, several species of Myxicola were described from California, Puget Sound, and Alaska. This material needs to be re-examined.</t>
   </si>
   <si>
     <t>367054</t>
@@ -4232,12 +4229,12 @@
         <v>36</v>
       </c>
       <c r="AH24" t="s">
-        <v>149</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B25" t="s">
         <v>35</v>
@@ -4288,25 +4285,25 @@
         <v>36</v>
       </c>
       <c r="R25" t="s">
+        <v>150</v>
+      </c>
+      <c r="S25" t="s">
+        <v>36</v>
+      </c>
+      <c r="T25" t="s">
         <v>151</v>
       </c>
-      <c r="S25" t="s">
-        <v>36</v>
-      </c>
-      <c r="T25" t="s">
+      <c r="U25" t="s">
         <v>152</v>
       </c>
-      <c r="U25" t="s">
+      <c r="V25" t="s">
+        <v>36</v>
+      </c>
+      <c r="W25" t="s">
+        <v>36</v>
+      </c>
+      <c r="X25" t="s">
         <v>153</v>
-      </c>
-      <c r="V25" t="s">
-        <v>36</v>
-      </c>
-      <c r="W25" t="s">
-        <v>36</v>
-      </c>
-      <c r="X25" t="s">
-        <v>154</v>
       </c>
       <c r="Y25" t="s">
         <v>36</v>
@@ -4341,7 +4338,7 @@
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B26" t="s">
         <v>35</v>
@@ -4380,37 +4377,37 @@
         <v>36</v>
       </c>
       <c r="N26" t="s">
+        <v>155</v>
+      </c>
+      <c r="O26" t="s">
+        <v>36</v>
+      </c>
+      <c r="P26" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>36</v>
+      </c>
+      <c r="R26" t="s">
         <v>156</v>
       </c>
-      <c r="O26" t="s">
-        <v>36</v>
-      </c>
-      <c r="P26" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>36</v>
-      </c>
-      <c r="R26" t="s">
+      <c r="S26" t="s">
+        <v>36</v>
+      </c>
+      <c r="T26" t="s">
         <v>157</v>
       </c>
-      <c r="S26" t="s">
-        <v>36</v>
-      </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
+        <v>36</v>
+      </c>
+      <c r="V26" t="s">
+        <v>36</v>
+      </c>
+      <c r="W26" t="s">
+        <v>36</v>
+      </c>
+      <c r="X26" t="s">
         <v>158</v>
-      </c>
-      <c r="U26" t="s">
-        <v>36</v>
-      </c>
-      <c r="V26" t="s">
-        <v>36</v>
-      </c>
-      <c r="W26" t="s">
-        <v>36</v>
-      </c>
-      <c r="X26" t="s">
-        <v>159</v>
       </c>
       <c r="Y26" t="s">
         <v>36</v>
@@ -4445,7 +4442,7 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
@@ -4472,49 +4469,49 @@
         <v>36</v>
       </c>
       <c r="J27" t="s">
+        <v>160</v>
+      </c>
+      <c r="K27" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" t="s">
+        <v>36</v>
+      </c>
+      <c r="M27" t="s">
+        <v>36</v>
+      </c>
+      <c r="N27" t="s">
         <v>161</v>
       </c>
-      <c r="K27" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" t="s">
-        <v>36</v>
-      </c>
-      <c r="M27" t="s">
-        <v>36</v>
-      </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>162</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>36</v>
+      </c>
+      <c r="R27" t="s">
         <v>163</v>
       </c>
-      <c r="P27" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>36</v>
-      </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
+        <v>36</v>
+      </c>
+      <c r="T27" t="s">
         <v>164</v>
       </c>
-      <c r="S27" t="s">
-        <v>36</v>
-      </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
+        <v>36</v>
+      </c>
+      <c r="V27" t="s">
+        <v>36</v>
+      </c>
+      <c r="W27" t="s">
+        <v>36</v>
+      </c>
+      <c r="X27" t="s">
         <v>165</v>
-      </c>
-      <c r="U27" t="s">
-        <v>36</v>
-      </c>
-      <c r="V27" t="s">
-        <v>36</v>
-      </c>
-      <c r="W27" t="s">
-        <v>36</v>
-      </c>
-      <c r="X27" t="s">
-        <v>166</v>
       </c>
       <c r="Y27" t="s">
         <v>36</v>
@@ -4549,7 +4546,7 @@
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
@@ -4576,23 +4573,23 @@
         <v>36</v>
       </c>
       <c r="J28" t="s">
+        <v>160</v>
+      </c>
+      <c r="K28" t="s">
+        <v>36</v>
+      </c>
+      <c r="L28" t="s">
+        <v>36</v>
+      </c>
+      <c r="M28" t="s">
+        <v>36</v>
+      </c>
+      <c r="N28" t="s">
         <v>161</v>
       </c>
-      <c r="K28" t="s">
-        <v>36</v>
-      </c>
-      <c r="L28" t="s">
-        <v>36</v>
-      </c>
-      <c r="M28" t="s">
-        <v>36</v>
-      </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>162</v>
       </c>
-      <c r="O28" t="s">
-        <v>163</v>
-      </c>
       <c r="P28" t="s">
         <v>36</v>
       </c>
@@ -4600,13 +4597,13 @@
         <v>36</v>
       </c>
       <c r="R28" t="s">
+        <v>167</v>
+      </c>
+      <c r="S28" t="s">
+        <v>36</v>
+      </c>
+      <c r="T28" t="s">
         <v>168</v>
-      </c>
-      <c r="S28" t="s">
-        <v>36</v>
-      </c>
-      <c r="T28" t="s">
-        <v>169</v>
       </c>
       <c r="U28" t="s">
         <v>36</v>
@@ -4653,7 +4650,7 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
@@ -4680,23 +4677,23 @@
         <v>36</v>
       </c>
       <c r="J29" t="s">
+        <v>160</v>
+      </c>
+      <c r="K29" t="s">
+        <v>36</v>
+      </c>
+      <c r="L29" t="s">
+        <v>36</v>
+      </c>
+      <c r="M29" t="s">
+        <v>36</v>
+      </c>
+      <c r="N29" t="s">
         <v>161</v>
       </c>
-      <c r="K29" t="s">
-        <v>36</v>
-      </c>
-      <c r="L29" t="s">
-        <v>36</v>
-      </c>
-      <c r="M29" t="s">
-        <v>36</v>
-      </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>162</v>
       </c>
-      <c r="O29" t="s">
-        <v>163</v>
-      </c>
       <c r="P29" t="s">
         <v>36</v>
       </c>
@@ -4704,25 +4701,25 @@
         <v>36</v>
       </c>
       <c r="R29" t="s">
+        <v>170</v>
+      </c>
+      <c r="S29" t="s">
+        <v>36</v>
+      </c>
+      <c r="T29" t="s">
         <v>171</v>
       </c>
-      <c r="S29" t="s">
-        <v>36</v>
-      </c>
-      <c r="T29" t="s">
+      <c r="U29" t="s">
+        <v>36</v>
+      </c>
+      <c r="V29" t="s">
+        <v>36</v>
+      </c>
+      <c r="W29" t="s">
+        <v>36</v>
+      </c>
+      <c r="X29" t="s">
         <v>172</v>
-      </c>
-      <c r="U29" t="s">
-        <v>36</v>
-      </c>
-      <c r="V29" t="s">
-        <v>36</v>
-      </c>
-      <c r="W29" t="s">
-        <v>36</v>
-      </c>
-      <c r="X29" t="s">
-        <v>173</v>
       </c>
       <c r="Y29" t="s">
         <v>36</v>
@@ -4757,7 +4754,7 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
@@ -4784,23 +4781,23 @@
         <v>36</v>
       </c>
       <c r="J30" t="s">
+        <v>160</v>
+      </c>
+      <c r="K30" t="s">
+        <v>36</v>
+      </c>
+      <c r="L30" t="s">
+        <v>36</v>
+      </c>
+      <c r="M30" t="s">
+        <v>36</v>
+      </c>
+      <c r="N30" t="s">
         <v>161</v>
       </c>
-      <c r="K30" t="s">
-        <v>36</v>
-      </c>
-      <c r="L30" t="s">
-        <v>36</v>
-      </c>
-      <c r="M30" t="s">
-        <v>36</v>
-      </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>162</v>
       </c>
-      <c r="O30" t="s">
-        <v>163</v>
-      </c>
       <c r="P30" t="s">
         <v>36</v>
       </c>
@@ -4808,17 +4805,17 @@
         <v>36</v>
       </c>
       <c r="R30" t="s">
+        <v>174</v>
+      </c>
+      <c r="S30" t="s">
+        <v>36</v>
+      </c>
+      <c r="T30" t="s">
         <v>175</v>
       </c>
-      <c r="S30" t="s">
-        <v>36</v>
-      </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>176</v>
       </c>
-      <c r="U30" t="s">
-        <v>36</v>
-      </c>
       <c r="V30" t="s">
         <v>36</v>
       </c>
@@ -4826,42 +4823,42 @@
         <v>36</v>
       </c>
       <c r="X30" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH30" t="s">
         <v>177</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH30" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
@@ -4888,23 +4885,23 @@
         <v>36</v>
       </c>
       <c r="J31" t="s">
+        <v>160</v>
+      </c>
+      <c r="K31" t="s">
+        <v>36</v>
+      </c>
+      <c r="L31" t="s">
+        <v>36</v>
+      </c>
+      <c r="M31" t="s">
+        <v>36</v>
+      </c>
+      <c r="N31" t="s">
         <v>161</v>
       </c>
-      <c r="K31" t="s">
-        <v>36</v>
-      </c>
-      <c r="L31" t="s">
-        <v>36</v>
-      </c>
-      <c r="M31" t="s">
-        <v>36</v>
-      </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>162</v>
       </c>
-      <c r="O31" t="s">
-        <v>163</v>
-      </c>
       <c r="P31" t="s">
         <v>36</v>
       </c>
@@ -4912,60 +4909,60 @@
         <v>36</v>
       </c>
       <c r="R31" t="s">
+        <v>174</v>
+      </c>
+      <c r="S31" t="s">
+        <v>36</v>
+      </c>
+      <c r="T31" t="s">
         <v>175</v>
       </c>
-      <c r="S31" t="s">
-        <v>36</v>
-      </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
+        <v>179</v>
+      </c>
+      <c r="V31" t="s">
+        <v>36</v>
+      </c>
+      <c r="W31" t="s">
+        <v>36</v>
+      </c>
+      <c r="X31" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH31" t="s">
         <v>180</v>
-      </c>
-      <c r="U31" t="s">
-        <v>36</v>
-      </c>
-      <c r="V31" t="s">
-        <v>36</v>
-      </c>
-      <c r="W31" t="s">
-        <v>36</v>
-      </c>
-      <c r="X31" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG31" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH31" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
@@ -4992,23 +4989,23 @@
         <v>36</v>
       </c>
       <c r="J32" t="s">
+        <v>160</v>
+      </c>
+      <c r="K32" t="s">
+        <v>36</v>
+      </c>
+      <c r="L32" t="s">
+        <v>36</v>
+      </c>
+      <c r="M32" t="s">
+        <v>36</v>
+      </c>
+      <c r="N32" t="s">
         <v>161</v>
       </c>
-      <c r="K32" t="s">
-        <v>36</v>
-      </c>
-      <c r="L32" t="s">
-        <v>36</v>
-      </c>
-      <c r="M32" t="s">
-        <v>36</v>
-      </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>162</v>
       </c>
-      <c r="O32" t="s">
-        <v>163</v>
-      </c>
       <c r="P32" t="s">
         <v>36</v>
       </c>
@@ -5016,25 +5013,25 @@
         <v>36</v>
       </c>
       <c r="R32" t="s">
+        <v>182</v>
+      </c>
+      <c r="S32" t="s">
+        <v>36</v>
+      </c>
+      <c r="T32" t="s">
         <v>183</v>
       </c>
-      <c r="S32" t="s">
-        <v>36</v>
-      </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
+        <v>36</v>
+      </c>
+      <c r="V32" t="s">
+        <v>36</v>
+      </c>
+      <c r="W32" t="s">
+        <v>36</v>
+      </c>
+      <c r="X32" t="s">
         <v>184</v>
-      </c>
-      <c r="U32" t="s">
-        <v>36</v>
-      </c>
-      <c r="V32" t="s">
-        <v>36</v>
-      </c>
-      <c r="W32" t="s">
-        <v>36</v>
-      </c>
-      <c r="X32" t="s">
-        <v>185</v>
       </c>
       <c r="Y32" t="s">
         <v>36</v>
@@ -5069,7 +5066,7 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
@@ -5096,23 +5093,23 @@
         <v>36</v>
       </c>
       <c r="J33" t="s">
+        <v>160</v>
+      </c>
+      <c r="K33" t="s">
+        <v>36</v>
+      </c>
+      <c r="L33" t="s">
+        <v>36</v>
+      </c>
+      <c r="M33" t="s">
+        <v>36</v>
+      </c>
+      <c r="N33" t="s">
         <v>161</v>
       </c>
-      <c r="K33" t="s">
-        <v>36</v>
-      </c>
-      <c r="L33" t="s">
-        <v>36</v>
-      </c>
-      <c r="M33" t="s">
-        <v>36</v>
-      </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>162</v>
       </c>
-      <c r="O33" t="s">
-        <v>163</v>
-      </c>
       <c r="P33" t="s">
         <v>36</v>
       </c>
@@ -5120,13 +5117,13 @@
         <v>36</v>
       </c>
       <c r="R33" t="s">
+        <v>186</v>
+      </c>
+      <c r="S33" t="s">
+        <v>36</v>
+      </c>
+      <c r="T33" t="s">
         <v>187</v>
-      </c>
-      <c r="S33" t="s">
-        <v>36</v>
-      </c>
-      <c r="T33" t="s">
-        <v>188</v>
       </c>
       <c r="U33" t="s">
         <v>36</v>
@@ -5173,7 +5170,7 @@
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -5200,23 +5197,23 @@
         <v>36</v>
       </c>
       <c r="J34" t="s">
+        <v>160</v>
+      </c>
+      <c r="K34" t="s">
+        <v>36</v>
+      </c>
+      <c r="L34" t="s">
+        <v>36</v>
+      </c>
+      <c r="M34" t="s">
+        <v>36</v>
+      </c>
+      <c r="N34" t="s">
         <v>161</v>
       </c>
-      <c r="K34" t="s">
-        <v>36</v>
-      </c>
-      <c r="L34" t="s">
-        <v>36</v>
-      </c>
-      <c r="M34" t="s">
-        <v>36</v>
-      </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>162</v>
       </c>
-      <c r="O34" t="s">
-        <v>163</v>
-      </c>
       <c r="P34" t="s">
         <v>36</v>
       </c>
@@ -5224,25 +5221,25 @@
         <v>36</v>
       </c>
       <c r="R34" t="s">
+        <v>189</v>
+      </c>
+      <c r="S34" t="s">
+        <v>36</v>
+      </c>
+      <c r="T34" t="s">
         <v>190</v>
       </c>
-      <c r="S34" t="s">
-        <v>36</v>
-      </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
+        <v>36</v>
+      </c>
+      <c r="V34" t="s">
+        <v>36</v>
+      </c>
+      <c r="W34" t="s">
+        <v>36</v>
+      </c>
+      <c r="X34" t="s">
         <v>191</v>
-      </c>
-      <c r="U34" t="s">
-        <v>36</v>
-      </c>
-      <c r="V34" t="s">
-        <v>36</v>
-      </c>
-      <c r="W34" t="s">
-        <v>36</v>
-      </c>
-      <c r="X34" t="s">
-        <v>192</v>
       </c>
       <c r="Y34" t="s">
         <v>36</v>
@@ -5277,7 +5274,7 @@
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -5304,7 +5301,7 @@
         <v>36</v>
       </c>
       <c r="J35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K35" t="s">
         <v>36</v>
@@ -5316,37 +5313,37 @@
         <v>36</v>
       </c>
       <c r="N35" t="s">
+        <v>193</v>
+      </c>
+      <c r="O35" t="s">
+        <v>36</v>
+      </c>
+      <c r="P35" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>36</v>
+      </c>
+      <c r="R35" t="s">
         <v>194</v>
       </c>
-      <c r="O35" t="s">
-        <v>36</v>
-      </c>
-      <c r="P35" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>36</v>
-      </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
+        <v>36</v>
+      </c>
+      <c r="T35" t="s">
         <v>195</v>
       </c>
-      <c r="S35" t="s">
-        <v>36</v>
-      </c>
-      <c r="T35" t="s">
+      <c r="U35" t="s">
+        <v>36</v>
+      </c>
+      <c r="V35" t="s">
+        <v>36</v>
+      </c>
+      <c r="W35" t="s">
+        <v>36</v>
+      </c>
+      <c r="X35" t="s">
         <v>196</v>
-      </c>
-      <c r="U35" t="s">
-        <v>36</v>
-      </c>
-      <c r="V35" t="s">
-        <v>36</v>
-      </c>
-      <c r="W35" t="s">
-        <v>36</v>
-      </c>
-      <c r="X35" t="s">
-        <v>197</v>
       </c>
       <c r="Y35" t="s">
         <v>36</v>
@@ -5381,7 +5378,7 @@
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -5408,7 +5405,7 @@
         <v>36</v>
       </c>
       <c r="J36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K36" t="s">
         <v>36</v>
@@ -5420,7 +5417,7 @@
         <v>36</v>
       </c>
       <c r="N36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O36" t="s">
         <v>36</v>
@@ -5432,13 +5429,13 @@
         <v>36</v>
       </c>
       <c r="R36" t="s">
+        <v>198</v>
+      </c>
+      <c r="S36" t="s">
+        <v>36</v>
+      </c>
+      <c r="T36" t="s">
         <v>199</v>
-      </c>
-      <c r="S36" t="s">
-        <v>36</v>
-      </c>
-      <c r="T36" t="s">
-        <v>200</v>
       </c>
       <c r="U36" t="s">
         <v>36</v>
@@ -5485,7 +5482,7 @@
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -5512,7 +5509,7 @@
         <v>36</v>
       </c>
       <c r="J37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K37" t="s">
         <v>36</v>
@@ -5524,7 +5521,7 @@
         <v>36</v>
       </c>
       <c r="N37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O37" t="s">
         <v>36</v>
@@ -5536,25 +5533,25 @@
         <v>36</v>
       </c>
       <c r="R37" t="s">
+        <v>201</v>
+      </c>
+      <c r="S37" t="s">
+        <v>36</v>
+      </c>
+      <c r="T37" t="s">
+        <v>164</v>
+      </c>
+      <c r="U37" t="s">
+        <v>36</v>
+      </c>
+      <c r="V37" t="s">
+        <v>36</v>
+      </c>
+      <c r="W37" t="s">
+        <v>36</v>
+      </c>
+      <c r="X37" t="s">
         <v>202</v>
-      </c>
-      <c r="S37" t="s">
-        <v>36</v>
-      </c>
-      <c r="T37" t="s">
-        <v>165</v>
-      </c>
-      <c r="U37" t="s">
-        <v>36</v>
-      </c>
-      <c r="V37" t="s">
-        <v>36</v>
-      </c>
-      <c r="W37" t="s">
-        <v>36</v>
-      </c>
-      <c r="X37" t="s">
-        <v>203</v>
       </c>
       <c r="Y37" t="s">
         <v>36</v>
@@ -5589,7 +5586,7 @@
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B38" t="s">
         <v>35</v>
@@ -5616,7 +5613,7 @@
         <v>36</v>
       </c>
       <c r="J38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K38" t="s">
         <v>36</v>
@@ -5628,7 +5625,7 @@
         <v>36</v>
       </c>
       <c r="N38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O38" t="s">
         <v>36</v>
@@ -5640,25 +5637,25 @@
         <v>36</v>
       </c>
       <c r="R38" t="s">
+        <v>204</v>
+      </c>
+      <c r="S38" t="s">
+        <v>36</v>
+      </c>
+      <c r="T38" t="s">
         <v>205</v>
       </c>
-      <c r="S38" t="s">
-        <v>36</v>
-      </c>
-      <c r="T38" t="s">
+      <c r="U38" t="s">
+        <v>36</v>
+      </c>
+      <c r="V38" t="s">
+        <v>36</v>
+      </c>
+      <c r="W38" t="s">
+        <v>36</v>
+      </c>
+      <c r="X38" t="s">
         <v>206</v>
-      </c>
-      <c r="U38" t="s">
-        <v>36</v>
-      </c>
-      <c r="V38" t="s">
-        <v>36</v>
-      </c>
-      <c r="W38" t="s">
-        <v>36</v>
-      </c>
-      <c r="X38" t="s">
-        <v>207</v>
       </c>
       <c r="Y38" t="s">
         <v>36</v>
@@ -5693,7 +5690,7 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
@@ -5720,7 +5717,7 @@
         <v>36</v>
       </c>
       <c r="J39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K39" t="s">
         <v>36</v>
@@ -5732,7 +5729,7 @@
         <v>36</v>
       </c>
       <c r="N39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O39" t="s">
         <v>36</v>
@@ -5744,25 +5741,25 @@
         <v>36</v>
       </c>
       <c r="R39" t="s">
+        <v>208</v>
+      </c>
+      <c r="S39" t="s">
+        <v>36</v>
+      </c>
+      <c r="T39" t="s">
         <v>209</v>
       </c>
-      <c r="S39" t="s">
-        <v>36</v>
-      </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
+        <v>36</v>
+      </c>
+      <c r="V39" t="s">
+        <v>36</v>
+      </c>
+      <c r="W39" t="s">
+        <v>36</v>
+      </c>
+      <c r="X39" t="s">
         <v>210</v>
-      </c>
-      <c r="U39" t="s">
-        <v>36</v>
-      </c>
-      <c r="V39" t="s">
-        <v>36</v>
-      </c>
-      <c r="W39" t="s">
-        <v>36</v>
-      </c>
-      <c r="X39" t="s">
-        <v>211</v>
       </c>
       <c r="Y39" t="s">
         <v>36</v>
@@ -5797,7 +5794,7 @@
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
@@ -5824,7 +5821,7 @@
         <v>36</v>
       </c>
       <c r="J40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K40" t="s">
         <v>36</v>
@@ -5836,7 +5833,7 @@
         <v>36</v>
       </c>
       <c r="N40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O40" t="s">
         <v>36</v>
@@ -5848,60 +5845,60 @@
         <v>36</v>
       </c>
       <c r="R40" t="s">
+        <v>212</v>
+      </c>
+      <c r="S40" t="s">
+        <v>36</v>
+      </c>
+      <c r="T40" t="s">
         <v>213</v>
       </c>
-      <c r="S40" t="s">
-        <v>36</v>
-      </c>
-      <c r="T40" t="s">
+      <c r="U40" t="s">
+        <v>36</v>
+      </c>
+      <c r="V40" t="s">
+        <v>36</v>
+      </c>
+      <c r="W40" t="s">
+        <v>36</v>
+      </c>
+      <c r="X40" t="s">
         <v>214</v>
       </c>
-      <c r="U40" t="s">
-        <v>36</v>
-      </c>
-      <c r="V40" t="s">
-        <v>36</v>
-      </c>
-      <c r="W40" t="s">
-        <v>36</v>
-      </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH40" t="s">
         <v>215</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH40" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B41" t="s">
         <v>35</v>
@@ -5928,7 +5925,7 @@
         <v>36</v>
       </c>
       <c r="J41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K41" t="s">
         <v>36</v>
@@ -5940,25 +5937,25 @@
         <v>36</v>
       </c>
       <c r="N41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O41" t="s">
+        <v>217</v>
+      </c>
+      <c r="P41" t="s">
         <v>218</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
+        <v>36</v>
+      </c>
+      <c r="R41" t="s">
         <v>219</v>
       </c>
-      <c r="Q41" t="s">
-        <v>36</v>
-      </c>
-      <c r="R41" t="s">
+      <c r="S41" t="s">
+        <v>36</v>
+      </c>
+      <c r="T41" t="s">
         <v>220</v>
-      </c>
-      <c r="S41" t="s">
-        <v>36</v>
-      </c>
-      <c r="T41" t="s">
-        <v>221</v>
       </c>
       <c r="U41" t="s">
         <v>36</v>
@@ -6005,7 +6002,7 @@
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B42" t="s">
         <v>35</v>
@@ -6032,38 +6029,38 @@
         <v>36</v>
       </c>
       <c r="J42" t="s">
+        <v>222</v>
+      </c>
+      <c r="K42" t="s">
         <v>223</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
+        <v>36</v>
+      </c>
+      <c r="M42" t="s">
+        <v>36</v>
+      </c>
+      <c r="N42" t="s">
         <v>224</v>
       </c>
-      <c r="L42" t="s">
-        <v>36</v>
-      </c>
-      <c r="M42" t="s">
-        <v>36</v>
-      </c>
-      <c r="N42" t="s">
+      <c r="O42" t="s">
+        <v>36</v>
+      </c>
+      <c r="P42" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>36</v>
+      </c>
+      <c r="R42" t="s">
         <v>225</v>
       </c>
-      <c r="O42" t="s">
-        <v>36</v>
-      </c>
-      <c r="P42" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>36</v>
-      </c>
-      <c r="R42" t="s">
+      <c r="S42" t="s">
+        <v>36</v>
+      </c>
+      <c r="T42" t="s">
         <v>226</v>
       </c>
-      <c r="S42" t="s">
-        <v>36</v>
-      </c>
-      <c r="T42" t="s">
-        <v>227</v>
-      </c>
       <c r="U42" t="s">
         <v>36</v>
       </c>
@@ -6074,7 +6071,7 @@
         <v>36</v>
       </c>
       <c r="X42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y42" t="s">
         <v>36</v>
@@ -6109,7 +6106,7 @@
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
@@ -6136,20 +6133,20 @@
         <v>36</v>
       </c>
       <c r="J43" t="s">
+        <v>222</v>
+      </c>
+      <c r="K43" t="s">
         <v>223</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
+        <v>36</v>
+      </c>
+      <c r="M43" t="s">
+        <v>36</v>
+      </c>
+      <c r="N43" t="s">
         <v>224</v>
       </c>
-      <c r="L43" t="s">
-        <v>36</v>
-      </c>
-      <c r="M43" t="s">
-        <v>36</v>
-      </c>
-      <c r="N43" t="s">
-        <v>225</v>
-      </c>
       <c r="O43" t="s">
         <v>36</v>
       </c>
@@ -6160,60 +6157,60 @@
         <v>36</v>
       </c>
       <c r="R43" t="s">
+        <v>228</v>
+      </c>
+      <c r="S43" t="s">
+        <v>36</v>
+      </c>
+      <c r="T43" t="s">
         <v>229</v>
       </c>
-      <c r="S43" t="s">
-        <v>36</v>
-      </c>
-      <c r="T43" t="s">
+      <c r="U43" t="s">
+        <v>36</v>
+      </c>
+      <c r="V43" t="s">
+        <v>36</v>
+      </c>
+      <c r="W43" t="s">
+        <v>36</v>
+      </c>
+      <c r="X43" t="s">
         <v>230</v>
       </c>
-      <c r="U43" t="s">
-        <v>36</v>
-      </c>
-      <c r="V43" t="s">
-        <v>36</v>
-      </c>
-      <c r="W43" t="s">
-        <v>36</v>
-      </c>
-      <c r="X43" t="s">
+      <c r="Y43" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH43" t="s">
         <v>231</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB43" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC43" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD43" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE43" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF43" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG43" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH43" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B44" t="s">
         <v>35</v>
@@ -6240,20 +6237,20 @@
         <v>36</v>
       </c>
       <c r="J44" t="s">
+        <v>222</v>
+      </c>
+      <c r="K44" t="s">
         <v>223</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
+        <v>36</v>
+      </c>
+      <c r="M44" t="s">
+        <v>36</v>
+      </c>
+      <c r="N44" t="s">
         <v>224</v>
       </c>
-      <c r="L44" t="s">
-        <v>36</v>
-      </c>
-      <c r="M44" t="s">
-        <v>36</v>
-      </c>
-      <c r="N44" t="s">
-        <v>225</v>
-      </c>
       <c r="O44" t="s">
         <v>36</v>
       </c>
@@ -6264,60 +6261,60 @@
         <v>36</v>
       </c>
       <c r="R44" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="S44" t="s">
         <v>36</v>
       </c>
       <c r="T44" t="s">
+        <v>233</v>
+      </c>
+      <c r="U44" t="s">
+        <v>36</v>
+      </c>
+      <c r="V44" t="s">
+        <v>36</v>
+      </c>
+      <c r="W44" t="s">
+        <v>36</v>
+      </c>
+      <c r="X44" t="s">
         <v>234</v>
       </c>
-      <c r="U44" t="s">
-        <v>36</v>
-      </c>
-      <c r="V44" t="s">
-        <v>36</v>
-      </c>
-      <c r="W44" t="s">
-        <v>36</v>
-      </c>
-      <c r="X44" t="s">
+      <c r="Y44" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH44" t="s">
         <v>235</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH44" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B45" t="s">
         <v>35</v>
@@ -6344,37 +6341,37 @@
         <v>36</v>
       </c>
       <c r="J45" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K45" t="s">
+        <v>237</v>
+      </c>
+      <c r="L45" t="s">
+        <v>36</v>
+      </c>
+      <c r="M45" t="s">
+        <v>36</v>
+      </c>
+      <c r="N45" t="s">
         <v>238</v>
       </c>
-      <c r="L45" t="s">
-        <v>36</v>
-      </c>
-      <c r="M45" t="s">
-        <v>36</v>
-      </c>
-      <c r="N45" t="s">
+      <c r="O45" t="s">
         <v>239</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>36</v>
+      </c>
+      <c r="R45" t="s">
         <v>240</v>
       </c>
-      <c r="P45" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>36</v>
-      </c>
-      <c r="R45" t="s">
+      <c r="S45" t="s">
+        <v>36</v>
+      </c>
+      <c r="T45" t="s">
         <v>241</v>
-      </c>
-      <c r="S45" t="s">
-        <v>36</v>
-      </c>
-      <c r="T45" t="s">
-        <v>242</v>
       </c>
       <c r="U45" t="s">
         <v>36</v>
@@ -6421,7 +6418,7 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B46" t="s">
         <v>35</v>
@@ -6448,23 +6445,23 @@
         <v>36</v>
       </c>
       <c r="J46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K46" t="s">
+        <v>237</v>
+      </c>
+      <c r="L46" t="s">
+        <v>36</v>
+      </c>
+      <c r="M46" t="s">
+        <v>36</v>
+      </c>
+      <c r="N46" t="s">
         <v>238</v>
       </c>
-      <c r="L46" t="s">
-        <v>36</v>
-      </c>
-      <c r="M46" t="s">
-        <v>36</v>
-      </c>
-      <c r="N46" t="s">
+      <c r="O46" t="s">
         <v>239</v>
       </c>
-      <c r="O46" t="s">
-        <v>240</v>
-      </c>
       <c r="P46" t="s">
         <v>36</v>
       </c>
@@ -6472,25 +6469,25 @@
         <v>36</v>
       </c>
       <c r="R46" t="s">
+        <v>243</v>
+      </c>
+      <c r="S46" t="s">
+        <v>36</v>
+      </c>
+      <c r="T46" t="s">
         <v>244</v>
       </c>
-      <c r="S46" t="s">
-        <v>36</v>
-      </c>
-      <c r="T46" t="s">
+      <c r="U46" t="s">
+        <v>36</v>
+      </c>
+      <c r="V46" t="s">
+        <v>36</v>
+      </c>
+      <c r="W46" t="s">
+        <v>36</v>
+      </c>
+      <c r="X46" t="s">
         <v>245</v>
-      </c>
-      <c r="U46" t="s">
-        <v>36</v>
-      </c>
-      <c r="V46" t="s">
-        <v>36</v>
-      </c>
-      <c r="W46" t="s">
-        <v>36</v>
-      </c>
-      <c r="X46" t="s">
-        <v>246</v>
       </c>
       <c r="Y46" t="s">
         <v>36</v>
@@ -6525,7 +6522,7 @@
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -6552,37 +6549,37 @@
         <v>36</v>
       </c>
       <c r="J47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K47" t="s">
+        <v>237</v>
+      </c>
+      <c r="L47" t="s">
+        <v>36</v>
+      </c>
+      <c r="M47" t="s">
+        <v>36</v>
+      </c>
+      <c r="N47" t="s">
         <v>238</v>
       </c>
-      <c r="L47" t="s">
-        <v>36</v>
-      </c>
-      <c r="M47" t="s">
-        <v>36</v>
-      </c>
-      <c r="N47" t="s">
-        <v>239</v>
-      </c>
       <c r="O47" t="s">
+        <v>247</v>
+      </c>
+      <c r="P47" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>36</v>
+      </c>
+      <c r="R47" t="s">
         <v>248</v>
       </c>
-      <c r="P47" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>36</v>
-      </c>
-      <c r="R47" t="s">
-        <v>249</v>
-      </c>
       <c r="S47" t="s">
         <v>36</v>
       </c>
       <c r="T47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U47" t="s">
         <v>36</v>
@@ -6640,472 +6637,472 @@
   <sheetData>
     <row r="1" spans="1:156" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" t="s">
         <v>250</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>251</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>252</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>253</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>254</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>255</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>256</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>257</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>258</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>259</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>260</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>261</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>262</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>263</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>264</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>265</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>266</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>267</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>268</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>269</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>270</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>271</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>272</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>273</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>274</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>275</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>276</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>277</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>278</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>279</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>280</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>281</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>282</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>283</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>284</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>285</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>286</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>287</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>288</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>289</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>290</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>291</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>292</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>293</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>294</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>295</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>296</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>297</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>298</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>299</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>300</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>301</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>302</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>303</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>304</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>305</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>306</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>307</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>308</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>309</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>310</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>311</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>312</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>313</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>314</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>315</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>316</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>317</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>318</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>319</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>320</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>321</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>322</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>323</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>324</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>325</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>326</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>327</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>328</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>329</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>330</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>331</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>332</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>333</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>334</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>335</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>336</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>337</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>338</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>339</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>340</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>341</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CP1" t="s">
         <v>342</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CQ1" t="s">
         <v>343</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>344</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CS1" t="s">
         <v>345</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CT1" t="s">
         <v>346</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CU1" t="s">
         <v>347</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CV1" t="s">
         <v>348</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CW1" t="s">
         <v>349</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>350</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>351</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>352</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>353</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>354</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DC1" t="s">
         <v>355</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DD1" t="s">
         <v>356</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" t="s">
         <v>357</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" t="s">
         <v>358</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DG1" t="s">
         <v>359</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DH1" t="s">
         <v>360</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DI1" t="s">
         <v>361</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DJ1" t="s">
         <v>362</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DK1" t="s">
         <v>363</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DL1" t="s">
         <v>364</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DM1" t="s">
         <v>365</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DN1" t="s">
         <v>366</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DO1" t="s">
         <v>367</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DP1" t="s">
         <v>368</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DQ1" t="s">
         <v>369</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DR1" t="s">
         <v>370</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="DS1" t="s">
         <v>371</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DT1" t="s">
         <v>372</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="DU1" t="s">
         <v>373</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
         <v>374</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DW1" t="s">
         <v>375</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DX1" t="s">
         <v>376</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="DY1" t="s">
         <v>377</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="DZ1" t="s">
         <v>378</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EA1" t="s">
         <v>379</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EB1" t="s">
         <v>380</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>381</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="ED1" t="s">
         <v>382</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EE1" t="s">
         <v>383</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EF1" t="s">
         <v>384</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EG1" t="s">
         <v>385</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EH1" t="s">
         <v>386</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EI1" t="s">
         <v>387</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EJ1" t="s">
         <v>388</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EK1" t="s">
         <v>389</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="EL1" t="s">
         <v>390</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EM1" t="s">
         <v>391</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EN1" t="s">
         <v>392</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="EO1" t="s">
         <v>393</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="EP1" t="s">
         <v>394</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="EQ1" t="s">
         <v>395</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ER1" t="s">
         <v>396</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="ES1" t="s">
         <v>397</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="ET1" t="s">
         <v>398</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="EU1" t="s">
         <v>399</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EV1" t="s">
         <v>400</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EW1" t="s">
         <v>401</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EX1" t="s">
         <v>402</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="EY1" t="s">
         <v>403</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="EZ1" t="s">
         <v>404</v>
-      </c>
-      <c r="EZ1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:156" x14ac:dyDescent="0.25">
@@ -7113,457 +7110,457 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C2" t="s">
         <v>406</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
         <v>407</v>
       </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
         <v>408</v>
       </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>409</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
         <v>410</v>
       </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
         <v>411</v>
       </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>36</v>
+      </c>
+      <c r="U2" t="s">
         <v>412</v>
       </c>
-      <c r="T2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
         <v>413</v>
       </c>
-      <c r="V2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
         <v>414</v>
       </c>
-      <c r="Y2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
         <v>415</v>
       </c>
-      <c r="AG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>416</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>417</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>418</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>419</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>420</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>421</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AX2" t="s">
         <v>422</v>
       </c>
-      <c r="AT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX2" t="s">
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ2" t="s">
         <v>423</v>
       </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ2" t="s">
+      <c r="BK2" t="s">
         <v>424</v>
       </c>
-      <c r="BK2" t="s">
+      <c r="BL2" t="s">
         <v>425</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BM2" t="s">
         <v>426</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP2" t="s">
         <v>427</v>
       </c>
-      <c r="BN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BP2" t="s">
+      <c r="BQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BU2" t="s">
         <v>428</v>
       </c>
-      <c r="BQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BU2" t="s">
+      <c r="BV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CG2" t="s">
         <v>429</v>
       </c>
-      <c r="BV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG2" t="s">
+      <c r="CH2" t="s">
         <v>430</v>
       </c>
-      <c r="CH2" t="s">
+      <c r="CI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CJ2" t="s">
         <v>431</v>
       </c>
-      <c r="CI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CJ2" t="s">
+      <c r="CK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>407</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY2" t="s">
         <v>432</v>
       </c>
-      <c r="CK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>408</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CY2" t="s">
+      <c r="CZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT2" t="s">
         <v>433</v>
       </c>
-      <c r="CZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DT2" t="s">
+      <c r="DU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DV2" t="s">
         <v>434</v>
       </c>
-      <c r="DU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DV2" t="s">
+      <c r="DW2" t="s">
         <v>435</v>
       </c>
-      <c r="DW2" t="s">
+      <c r="DX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DZ2" t="s">
         <v>436</v>
       </c>
-      <c r="DX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DZ2" t="s">
+      <c r="EA2" t="s">
         <v>437</v>
       </c>
-      <c r="EA2" t="s">
+      <c r="EB2" t="s">
         <v>438</v>
       </c>
-      <c r="EB2" t="s">
+      <c r="EC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EE2" t="s">
         <v>439</v>
       </c>
-      <c r="EC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EE2" t="s">
+      <c r="EF2" t="s">
         <v>440</v>
       </c>
-      <c r="EF2" t="s">
+      <c r="EG2" t="s">
         <v>441</v>
       </c>
-      <c r="EG2" t="s">
+      <c r="EH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>412</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ER2" t="s">
         <v>442</v>
       </c>
-      <c r="EH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>413</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ER2" t="s">
+      <c r="ES2" t="s">
         <v>443</v>
       </c>
-      <c r="ES2" t="s">
+      <c r="ET2" t="s">
         <v>444</v>
       </c>
-      <c r="ET2" t="s">
+      <c r="EU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EV2" t="s">
         <v>445</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>446</v>
       </c>
       <c r="EW2" t="s">
         <v>36</v>
@@ -7594,10 +7591,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C1" t="s">
         <v>447</v>
-      </c>
-      <c r="C1" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>